<commit_message>
Big old mess I need to hide for a bit
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="15">
   <si>
     <t>Mode</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>AES</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -389,7 +392,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -440,42 +443,42 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>192</v>
+        <v>128</v>
       </c>
       <c r="D3">
         <v>10</v>
       </c>
       <c r="E3">
-        <v>8685014</v>
+        <v>480175367</v>
       </c>
       <c r="F3">
-        <v>26</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C4">
-        <v>192</v>
+        <v>128</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4">
-        <v>12507639</v>
+        <v>7645256</v>
       </c>
       <c r="F4">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -483,7 +486,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>128</v>
@@ -492,15 +495,18 @@
         <v>10</v>
       </c>
       <c r="E5">
-        <v>480175367</v>
+        <v>5932714</v>
       </c>
       <c r="F5">
-        <v>124</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
       </c>
       <c r="C6">
         <v>128</v>
@@ -509,30 +515,30 @@
         <v>10</v>
       </c>
       <c r="E6">
-        <v>7645256</v>
+        <v>14373081</v>
       </c>
       <c r="F6">
-        <v>125</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="D7">
         <v>10</v>
       </c>
       <c r="E7">
-        <v>16605503</v>
+        <v>6116200</v>
       </c>
       <c r="F7">
-        <v>137</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -540,7 +546,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>128</v>
@@ -549,10 +555,10 @@
         <v>10</v>
       </c>
       <c r="E8">
-        <v>5932714</v>
+        <v>11223237</v>
       </c>
       <c r="F8">
-        <v>149</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -560,7 +566,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>128</v>
@@ -569,30 +575,30 @@
         <v>10</v>
       </c>
       <c r="E9">
-        <v>14373081</v>
+        <v>13944946</v>
       </c>
       <c r="F9">
-        <v>154</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
-        <v>192</v>
+        <v>128</v>
       </c>
       <c r="D10">
         <v>10</v>
       </c>
       <c r="E10">
-        <v>16727827</v>
+        <v>10886846</v>
       </c>
       <c r="F10">
-        <v>157</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -600,47 +606,47 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C11">
-        <v>192</v>
+        <v>128</v>
       </c>
       <c r="D11">
         <v>10</v>
       </c>
       <c r="E11">
-        <v>16422017</v>
+        <v>2856957157</v>
       </c>
       <c r="F11">
-        <v>158</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="D12">
         <v>10</v>
       </c>
       <c r="E12">
-        <v>13058097</v>
+        <v>6911307</v>
       </c>
       <c r="F12">
-        <v>161</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>192</v>
@@ -649,70 +655,70 @@
         <v>10</v>
       </c>
       <c r="E13">
-        <v>12293572</v>
+        <v>8685014</v>
       </c>
       <c r="F13">
-        <v>164</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14">
-        <v>256</v>
+        <v>192</v>
       </c>
       <c r="D14">
         <v>10</v>
       </c>
       <c r="E14">
-        <v>17003056</v>
+        <v>12507639</v>
       </c>
       <c r="F14">
-        <v>164</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15">
-        <v>128</v>
+        <v>192</v>
       </c>
       <c r="D15">
         <v>10</v>
       </c>
       <c r="E15">
-        <v>6116200</v>
+        <v>16727827</v>
       </c>
       <c r="F15">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C16">
-        <v>256</v>
+        <v>192</v>
       </c>
       <c r="D16">
         <v>10</v>
       </c>
       <c r="E16">
-        <v>3870182520</v>
+        <v>16422017</v>
       </c>
       <c r="F16">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -720,19 +726,19 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C17">
-        <v>128</v>
+        <v>192</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17">
-        <v>11223237</v>
+        <v>12293572</v>
       </c>
       <c r="F17">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -740,24 +746,24 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C18">
-        <v>128</v>
+        <v>192</v>
       </c>
       <c r="D18">
         <v>10</v>
       </c>
       <c r="E18">
-        <v>13944946</v>
+        <v>2406526010</v>
       </c>
       <c r="F18">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
@@ -769,10 +775,10 @@
         <v>10</v>
       </c>
       <c r="E19">
-        <v>2406526010</v>
+        <v>27389486</v>
       </c>
       <c r="F19">
-        <v>175</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -780,19 +786,19 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20">
-        <v>256</v>
+        <v>192</v>
       </c>
       <c r="D20">
         <v>10</v>
       </c>
       <c r="E20">
-        <v>12935773</v>
+        <v>6269105</v>
       </c>
       <c r="F20">
-        <v>179</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -800,19 +806,19 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C21">
-        <v>256</v>
+        <v>192</v>
       </c>
       <c r="D21">
         <v>10</v>
       </c>
       <c r="E21">
-        <v>1952945020</v>
+        <v>7247698</v>
       </c>
       <c r="F21">
-        <v>186</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -820,87 +826,87 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C22">
-        <v>128</v>
+        <v>192</v>
       </c>
       <c r="D22">
         <v>10</v>
       </c>
       <c r="E22">
-        <v>10886846</v>
+        <v>6422010</v>
       </c>
       <c r="F22">
-        <v>196</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C23">
-        <v>192</v>
+        <v>256</v>
       </c>
       <c r="D23">
         <v>10</v>
       </c>
       <c r="E23">
-        <v>27389486</v>
+        <v>16605503</v>
       </c>
       <c r="F23">
-        <v>197</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C24">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="D24">
         <v>10</v>
       </c>
       <c r="E24">
-        <v>2856957157</v>
+        <v>13058097</v>
       </c>
       <c r="F24">
-        <v>203</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C25">
-        <v>192</v>
+        <v>256</v>
       </c>
       <c r="D25">
         <v>10</v>
       </c>
       <c r="E25">
-        <v>6269105</v>
+        <v>17003056</v>
       </c>
       <c r="F25">
-        <v>206</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C26">
         <v>256</v>
@@ -909,30 +915,30 @@
         <v>10</v>
       </c>
       <c r="E26">
-        <v>7278279</v>
+        <v>3870182520</v>
       </c>
       <c r="F26">
-        <v>206</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C27">
-        <v>192</v>
+        <v>256</v>
       </c>
       <c r="D27">
         <v>10</v>
       </c>
       <c r="E27">
-        <v>7247698</v>
+        <v>12935773</v>
       </c>
       <c r="F27">
-        <v>209</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -940,47 +946,47 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C28">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="D28">
         <v>10</v>
       </c>
       <c r="E28">
-        <v>6911307</v>
+        <v>1952945020</v>
       </c>
       <c r="F28">
-        <v>256</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C29">
-        <v>192</v>
+        <v>256</v>
       </c>
       <c r="D29">
         <v>10</v>
       </c>
       <c r="E29">
-        <v>6422010</v>
+        <v>7278279</v>
       </c>
       <c r="F29">
-        <v>256</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C30">
         <v>256</v>
@@ -989,7 +995,7 @@
         <v>10</v>
       </c>
       <c r="E30">
-        <v>7217116</v>
+        <v>6207943</v>
       </c>
       <c r="F30">
         <v>256</v>
@@ -1000,7 +1006,7 @@
         <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C31">
         <v>256</v>
@@ -1009,7 +1015,7 @@
         <v>10</v>
       </c>
       <c r="E31">
-        <v>6207943</v>
+        <v>6422010</v>
       </c>
       <c r="F31">
         <v>256</v>
@@ -1017,7 +1023,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
@@ -1029,7 +1035,7 @@
         <v>10</v>
       </c>
       <c r="E32">
-        <v>6422010</v>
+        <v>7217116</v>
       </c>
       <c r="F32">
         <v>256</v>
@@ -1038,7 +1044,7 @@
   </sheetData>
   <autoFilter ref="A1:F1">
     <sortState ref="A2:F32">
-      <sortCondition ref="F1:F32"/>
+      <sortCondition ref="C1:C32"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>